<commit_message>
Computing accpeted papers with JCR > 1.5
</commit_message>
<xml_diff>
--- a/pgc.xlsx
+++ b/pgc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>Nome</t>
   </si>
@@ -167,6 +167,24 @@
   </si>
   <si>
     <t>Publicações Indexadas JCR &gt;= 1,5</t>
+  </si>
+  <si>
+    <t>Publicações JCR (total)</t>
+  </si>
+  <si>
+    <t>Publicações JCR &gt; 1,5 (total)</t>
+  </si>
+  <si>
+    <t>Publicações JCR</t>
+  </si>
+  <si>
+    <t>Publicações JCR &gt; 1,5</t>
+  </si>
+  <si>
+    <t>Aceitações JCR &gt; 1,5</t>
+  </si>
+  <si>
+    <t>Artigos JCR &gt; 1,5</t>
   </si>
   <si>
     <t>Alexandre Plastino de Carvalho</t>
@@ -872,13 +890,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY40"/>
+  <dimension ref="A1:BE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:57">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1032,16 +1050,34 @@
       <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AZ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:57">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D2">
         <v>2000</v>
@@ -1128,13 +1164,13 @@
         <v>22</v>
       </c>
       <c r="AF2">
-        <v>756</v>
+        <v>762</v>
       </c>
       <c r="AG2">
         <v>15</v>
       </c>
       <c r="AH2">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="AI2">
         <v>0.1111111111111111</v>
@@ -1176,7 +1212,7 @@
         <v>5.777777777777778</v>
       </c>
       <c r="AV2">
-        <v>42</v>
+        <v>42.33333333333334</v>
       </c>
       <c r="AW2">
         <v>0.8333333333333334</v>
@@ -1187,16 +1223,34 @@
       <c r="AY2">
         <v>4</v>
       </c>
+      <c r="AZ2">
+        <v>18</v>
+      </c>
+      <c r="BA2">
+        <v>11</v>
+      </c>
+      <c r="BB2">
+        <v>8</v>
+      </c>
+      <c r="BC2">
+        <v>4</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:57">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D3">
         <v>2011</v>
@@ -1342,16 +1396,34 @@
       <c r="AY3">
         <v>2</v>
       </c>
+      <c r="AZ3">
+        <v>4</v>
+      </c>
+      <c r="BA3">
+        <v>3</v>
+      </c>
+      <c r="BB3">
+        <v>3</v>
+      </c>
+      <c r="BC3">
+        <v>2</v>
+      </c>
+      <c r="BD3">
+        <v>0</v>
+      </c>
+      <c r="BE3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:57">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D4">
         <v>2003</v>
@@ -1497,16 +1569,34 @@
       <c r="AY4">
         <v>0</v>
       </c>
+      <c r="AZ4">
+        <v>5</v>
+      </c>
+      <c r="BA4">
+        <v>3</v>
+      </c>
+      <c r="BB4">
+        <v>1</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>0</v>
+      </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:57">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D5">
         <v>2010</v>
@@ -1652,16 +1742,34 @@
       <c r="AY5">
         <v>0</v>
       </c>
+      <c r="AZ5">
+        <v>4</v>
+      </c>
+      <c r="BA5">
+        <v>4</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5">
+        <v>0</v>
+      </c>
+      <c r="BE5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:57">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D6">
         <v>1988</v>
@@ -1748,13 +1856,13 @@
         <v>41</v>
       </c>
       <c r="AF6">
-        <v>2423</v>
+        <v>2425</v>
       </c>
       <c r="AG6">
         <v>27</v>
       </c>
       <c r="AH6">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="AI6">
         <v>0.4</v>
@@ -1796,7 +1904,7 @@
         <v>9.033333333333333</v>
       </c>
       <c r="AV6">
-        <v>80.76666666666667</v>
+        <v>80.83333333333333</v>
       </c>
       <c r="AW6">
         <v>0.9</v>
@@ -1807,16 +1915,34 @@
       <c r="AY6">
         <v>7</v>
       </c>
+      <c r="AZ6">
+        <v>34</v>
+      </c>
+      <c r="BA6">
+        <v>24</v>
+      </c>
+      <c r="BB6">
+        <v>11</v>
+      </c>
+      <c r="BC6">
+        <v>7</v>
+      </c>
+      <c r="BD6">
+        <v>1</v>
+      </c>
+      <c r="BE6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:57">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D7">
         <v>2014</v>
@@ -1962,16 +2088,34 @@
       <c r="AY7">
         <v>0</v>
       </c>
+      <c r="AZ7">
+        <v>2</v>
+      </c>
+      <c r="BA7">
+        <v>1</v>
+      </c>
+      <c r="BB7">
+        <v>1</v>
+      </c>
+      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="BD7">
+        <v>0</v>
+      </c>
+      <c r="BE7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:57">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D8">
         <v>1998</v>
@@ -2117,16 +2261,34 @@
       <c r="AY8">
         <v>1</v>
       </c>
+      <c r="AZ8">
+        <v>11</v>
+      </c>
+      <c r="BA8">
+        <v>4</v>
+      </c>
+      <c r="BB8">
+        <v>1</v>
+      </c>
+      <c r="BC8">
+        <v>1</v>
+      </c>
+      <c r="BD8">
+        <v>1</v>
+      </c>
+      <c r="BE8">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:57">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D9">
         <v>2000</v>
@@ -2213,13 +2375,13 @@
         <v>27</v>
       </c>
       <c r="AF9">
-        <v>2111</v>
+        <v>2113</v>
       </c>
       <c r="AG9">
         <v>22</v>
       </c>
       <c r="AH9">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="AI9">
         <v>0.4444444444444444</v>
@@ -2261,7 +2423,7 @@
         <v>8.111111111111111</v>
       </c>
       <c r="AV9">
-        <v>117.2777777777778</v>
+        <v>117.3888888888889</v>
       </c>
       <c r="AW9">
         <v>1.222222222222222</v>
@@ -2272,16 +2434,34 @@
       <c r="AY9">
         <v>4</v>
       </c>
+      <c r="AZ9">
+        <v>21</v>
+      </c>
+      <c r="BA9">
+        <v>17</v>
+      </c>
+      <c r="BB9">
+        <v>5</v>
+      </c>
+      <c r="BC9">
+        <v>4</v>
+      </c>
+      <c r="BD9">
+        <v>0</v>
+      </c>
+      <c r="BE9">
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:57">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D10">
         <v>1983</v>
@@ -2368,13 +2548,13 @@
         <v>17</v>
       </c>
       <c r="AF10">
-        <v>9119</v>
+        <v>9121</v>
       </c>
       <c r="AG10">
         <v>47</v>
       </c>
       <c r="AH10">
-        <v>1523</v>
+        <v>1526</v>
       </c>
       <c r="AI10">
         <v>0</v>
@@ -2416,7 +2596,7 @@
         <v>5.571428571428571</v>
       </c>
       <c r="AV10">
-        <v>260.5428571428571</v>
+        <v>260.6</v>
       </c>
       <c r="AW10">
         <v>1.342857142857143</v>
@@ -2427,16 +2607,34 @@
       <c r="AY10">
         <v>10</v>
       </c>
+      <c r="AZ10">
+        <v>93</v>
+      </c>
+      <c r="BA10">
+        <v>56</v>
+      </c>
+      <c r="BB10">
+        <v>11</v>
+      </c>
+      <c r="BC10">
+        <v>10</v>
+      </c>
+      <c r="BD10">
+        <v>1</v>
+      </c>
+      <c r="BE10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="11" spans="1:51">
+    <row r="11" spans="1:57">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D11">
         <v>2001</v>
@@ -2523,13 +2721,13 @@
         <v>7</v>
       </c>
       <c r="AF11">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="AG11">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AH11">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AI11">
         <v>1.294117647058824</v>
@@ -2571,10 +2769,10 @@
         <v>3.058823529411764</v>
       </c>
       <c r="AV11">
-        <v>39.88235294117647</v>
+        <v>39.76470588235294</v>
       </c>
       <c r="AW11">
-        <v>0.9411764705882353</v>
+        <v>0.8823529411764706</v>
       </c>
       <c r="AX11">
         <v>2</v>
@@ -2582,16 +2780,34 @@
       <c r="AY11">
         <v>0</v>
       </c>
+      <c r="AZ11">
+        <v>5</v>
+      </c>
+      <c r="BA11">
+        <v>2</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
+      <c r="BC11">
+        <v>0</v>
+      </c>
+      <c r="BD11">
+        <v>0</v>
+      </c>
+      <c r="BE11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:51">
+    <row r="12" spans="1:57">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D12">
         <v>2009</v>
@@ -2737,16 +2953,34 @@
       <c r="AY12">
         <v>0</v>
       </c>
+      <c r="AZ12">
+        <v>0</v>
+      </c>
+      <c r="BA12">
+        <v>0</v>
+      </c>
+      <c r="BB12">
+        <v>0</v>
+      </c>
+      <c r="BC12">
+        <v>0</v>
+      </c>
+      <c r="BD12">
+        <v>1</v>
+      </c>
+      <c r="BE12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:51">
+    <row r="13" spans="1:57">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D13">
         <v>2012</v>
@@ -2833,13 +3067,13 @@
         <v>49</v>
       </c>
       <c r="AF13">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="AG13">
         <v>22</v>
       </c>
       <c r="AH13">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AI13">
         <v>1.833333333333333</v>
@@ -2881,7 +3115,7 @@
         <v>25.5</v>
       </c>
       <c r="AV13">
-        <v>329.5</v>
+        <v>329.1666666666667</v>
       </c>
       <c r="AW13">
         <v>3.666666666666667</v>
@@ -2892,16 +3126,34 @@
       <c r="AY13">
         <v>6</v>
       </c>
+      <c r="AZ13">
+        <v>17</v>
+      </c>
+      <c r="BA13">
+        <v>11</v>
+      </c>
+      <c r="BB13">
+        <v>8</v>
+      </c>
+      <c r="BC13">
+        <v>6</v>
+      </c>
+      <c r="BD13">
+        <v>1</v>
+      </c>
+      <c r="BE13">
+        <v>7</v>
+      </c>
     </row>
-    <row r="14" spans="1:51">
+    <row r="14" spans="1:57">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D14">
         <v>2006</v>
@@ -3047,16 +3299,34 @@
       <c r="AY14">
         <v>0</v>
       </c>
+      <c r="AZ14">
+        <v>4</v>
+      </c>
+      <c r="BA14">
+        <v>2</v>
+      </c>
+      <c r="BB14">
+        <v>0</v>
+      </c>
+      <c r="BC14">
+        <v>0</v>
+      </c>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+      <c r="BE14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:51">
+    <row r="15" spans="1:57">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D15">
         <v>2003</v>
@@ -3143,13 +3413,13 @@
         <v>29</v>
       </c>
       <c r="AF15">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="AG15">
         <v>17</v>
       </c>
       <c r="AH15">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI15">
         <v>1.133333333333333</v>
@@ -3191,7 +3461,7 @@
         <v>9</v>
       </c>
       <c r="AV15">
-        <v>103.7333333333333</v>
+        <v>103.8</v>
       </c>
       <c r="AW15">
         <v>1.133333333333333</v>
@@ -3202,16 +3472,34 @@
       <c r="AY15">
         <v>2</v>
       </c>
+      <c r="AZ15">
+        <v>14</v>
+      </c>
+      <c r="BA15">
+        <v>9</v>
+      </c>
+      <c r="BB15">
+        <v>3</v>
+      </c>
+      <c r="BC15">
+        <v>2</v>
+      </c>
+      <c r="BD15">
+        <v>1</v>
+      </c>
+      <c r="BE15">
+        <v>3</v>
+      </c>
     </row>
-    <row r="16" spans="1:51">
+    <row r="16" spans="1:57">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D16">
         <v>2013</v>
@@ -3357,16 +3645,34 @@
       <c r="AY16">
         <v>3</v>
       </c>
+      <c r="AZ16">
+        <v>11</v>
+      </c>
+      <c r="BA16">
+        <v>11</v>
+      </c>
+      <c r="BB16">
+        <v>3</v>
+      </c>
+      <c r="BC16">
+        <v>3</v>
+      </c>
+      <c r="BD16">
+        <v>0</v>
+      </c>
+      <c r="BE16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:51">
+    <row r="17" spans="1:57">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D17">
         <v>2004</v>
@@ -3453,13 +3759,13 @@
         <v>49</v>
       </c>
       <c r="AF17">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="AG17">
         <v>20</v>
       </c>
       <c r="AH17">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="AI17">
         <v>0.2857142857142857</v>
@@ -3501,7 +3807,7 @@
         <v>15.57142857142857</v>
       </c>
       <c r="AV17">
-        <v>107.2142857142857</v>
+        <v>107.2857142857143</v>
       </c>
       <c r="AW17">
         <v>1.428571428571429</v>
@@ -3512,16 +3818,34 @@
       <c r="AY17">
         <v>3</v>
       </c>
+      <c r="AZ17">
+        <v>12</v>
+      </c>
+      <c r="BA17">
+        <v>7</v>
+      </c>
+      <c r="BB17">
+        <v>6</v>
+      </c>
+      <c r="BC17">
+        <v>3</v>
+      </c>
+      <c r="BD17">
+        <v>0</v>
+      </c>
+      <c r="BE17">
+        <v>3</v>
+      </c>
     </row>
-    <row r="18" spans="1:51">
+    <row r="18" spans="1:57">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D18">
         <v>1996</v>
@@ -3608,13 +3932,13 @@
         <v>8</v>
       </c>
       <c r="AF18">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="AG18">
         <v>14</v>
       </c>
       <c r="AH18">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI18">
         <v>0.5</v>
@@ -3656,7 +3980,7 @@
         <v>2.772727272727273</v>
       </c>
       <c r="AV18">
-        <v>28.77272727272727</v>
+        <v>28.81818181818182</v>
       </c>
       <c r="AW18">
         <v>0.6363636363636364</v>
@@ -3667,16 +3991,34 @@
       <c r="AY18">
         <v>1</v>
       </c>
+      <c r="AZ18">
+        <v>8</v>
+      </c>
+      <c r="BA18">
+        <v>3</v>
+      </c>
+      <c r="BB18">
+        <v>1</v>
+      </c>
+      <c r="BC18">
+        <v>1</v>
+      </c>
+      <c r="BD18">
+        <v>0</v>
+      </c>
+      <c r="BE18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:51">
+    <row r="19" spans="1:57">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D19">
         <v>1998</v>
@@ -3763,13 +4105,13 @@
         <v>24</v>
       </c>
       <c r="AF19">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="AG19">
         <v>17</v>
       </c>
       <c r="AH19">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AI19">
         <v>0.1</v>
@@ -3811,7 +4153,7 @@
         <v>6.3</v>
       </c>
       <c r="AV19">
-        <v>58.2</v>
+        <v>58.25</v>
       </c>
       <c r="AW19">
         <v>0.85</v>
@@ -3822,16 +4164,34 @@
       <c r="AY19">
         <v>4</v>
       </c>
+      <c r="AZ19">
+        <v>56</v>
+      </c>
+      <c r="BA19">
+        <v>11</v>
+      </c>
+      <c r="BB19">
+        <v>15</v>
+      </c>
+      <c r="BC19">
+        <v>4</v>
+      </c>
+      <c r="BD19">
+        <v>0</v>
+      </c>
+      <c r="BE19">
+        <v>4</v>
+      </c>
     </row>
-    <row r="20" spans="1:51">
+    <row r="20" spans="1:57">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D20">
         <v>2009</v>
@@ -3918,13 +4278,13 @@
         <v>14</v>
       </c>
       <c r="AF20">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="AG20">
         <v>14</v>
       </c>
       <c r="AH20">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AI20">
         <v>2.777777777777778</v>
@@ -3966,7 +4326,7 @@
         <v>7.888888888888889</v>
       </c>
       <c r="AV20">
-        <v>136.5555555555555</v>
+        <v>136.6666666666667</v>
       </c>
       <c r="AW20">
         <v>1.555555555555556</v>
@@ -3977,13 +4337,31 @@
       <c r="AY20">
         <v>1</v>
       </c>
+      <c r="AZ20">
+        <v>15</v>
+      </c>
+      <c r="BA20">
+        <v>8</v>
+      </c>
+      <c r="BB20">
+        <v>3</v>
+      </c>
+      <c r="BC20">
+        <v>1</v>
+      </c>
+      <c r="BD20">
+        <v>0</v>
+      </c>
+      <c r="BE20">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:51">
+    <row r="21" spans="1:57">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D21">
         <v>1989</v>
@@ -4114,16 +4492,34 @@
       <c r="AY21">
         <v>0</v>
       </c>
+      <c r="AZ21">
+        <v>14</v>
+      </c>
+      <c r="BA21">
+        <v>9</v>
+      </c>
+      <c r="BB21">
+        <v>2</v>
+      </c>
+      <c r="BC21">
+        <v>0</v>
+      </c>
+      <c r="BD21">
+        <v>0</v>
+      </c>
+      <c r="BE21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:51">
+    <row r="22" spans="1:57">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D22">
         <v>2009</v>
@@ -4210,13 +4606,13 @@
         <v>43</v>
       </c>
       <c r="AF22">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AG22">
         <v>11</v>
       </c>
       <c r="AH22">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AI22">
         <v>0.6666666666666666</v>
@@ -4258,7 +4654,7 @@
         <v>9.555555555555555</v>
       </c>
       <c r="AV22">
-        <v>49.77777777777778</v>
+        <v>49.88888888888889</v>
       </c>
       <c r="AW22">
         <v>1.222222222222222</v>
@@ -4269,16 +4665,34 @@
       <c r="AY22">
         <v>1</v>
       </c>
+      <c r="AZ22">
+        <v>4</v>
+      </c>
+      <c r="BA22">
+        <v>4</v>
+      </c>
+      <c r="BB22">
+        <v>1</v>
+      </c>
+      <c r="BC22">
+        <v>1</v>
+      </c>
+      <c r="BD22">
+        <v>0</v>
+      </c>
+      <c r="BE22">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:51">
+    <row r="23" spans="1:57">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D23">
         <v>1996</v>
@@ -4365,13 +4779,13 @@
         <v>13</v>
       </c>
       <c r="AF23">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="AG23">
         <v>26</v>
       </c>
       <c r="AH23">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="AI23">
         <v>0.1363636363636364</v>
@@ -4413,7 +4827,7 @@
         <v>7.590909090909091</v>
       </c>
       <c r="AV23">
-        <v>100.0454545454545</v>
+        <v>100</v>
       </c>
       <c r="AW23">
         <v>1.181818181818182</v>
@@ -4424,16 +4838,34 @@
       <c r="AY23">
         <v>3</v>
       </c>
+      <c r="AZ23">
+        <v>22</v>
+      </c>
+      <c r="BA23">
+        <v>21</v>
+      </c>
+      <c r="BB23">
+        <v>3</v>
+      </c>
+      <c r="BC23">
+        <v>3</v>
+      </c>
+      <c r="BD23">
+        <v>1</v>
+      </c>
+      <c r="BE23">
+        <v>4</v>
+      </c>
     </row>
-    <row r="24" spans="1:51">
+    <row r="24" spans="1:57">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D24">
         <v>2010</v>
@@ -4520,13 +4952,13 @@
         <v>5</v>
       </c>
       <c r="AF24">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="AG24">
         <v>8</v>
       </c>
       <c r="AH24">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AI24">
         <v>0.75</v>
@@ -4568,7 +5000,7 @@
         <v>3.75</v>
       </c>
       <c r="AV24">
-        <v>93.875</v>
+        <v>94</v>
       </c>
       <c r="AW24">
         <v>1</v>
@@ -4579,16 +5011,34 @@
       <c r="AY24">
         <v>1</v>
       </c>
+      <c r="AZ24">
+        <v>9</v>
+      </c>
+      <c r="BA24">
+        <v>8</v>
+      </c>
+      <c r="BB24">
+        <v>1</v>
+      </c>
+      <c r="BC24">
+        <v>1</v>
+      </c>
+      <c r="BD24">
+        <v>0</v>
+      </c>
+      <c r="BE24">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:51">
+    <row r="25" spans="1:57">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D25">
         <v>2006</v>
@@ -4675,13 +5125,13 @@
         <v>26</v>
       </c>
       <c r="AF25">
-        <v>1805</v>
+        <v>1803</v>
       </c>
       <c r="AG25">
         <v>22</v>
       </c>
       <c r="AH25">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="AI25">
         <v>1.166666666666667</v>
@@ -4723,7 +5173,7 @@
         <v>14.41666666666667</v>
       </c>
       <c r="AV25">
-        <v>150.4166666666667</v>
+        <v>150.25</v>
       </c>
       <c r="AW25">
         <v>1.833333333333333</v>
@@ -4734,16 +5184,34 @@
       <c r="AY25">
         <v>7</v>
       </c>
+      <c r="AZ25">
+        <v>18</v>
+      </c>
+      <c r="BA25">
+        <v>11</v>
+      </c>
+      <c r="BB25">
+        <v>8</v>
+      </c>
+      <c r="BC25">
+        <v>7</v>
+      </c>
+      <c r="BD25">
+        <v>1</v>
+      </c>
+      <c r="BE25">
+        <v>8</v>
+      </c>
     </row>
-    <row r="26" spans="1:51">
+    <row r="26" spans="1:57">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D26">
         <v>2003</v>
@@ -4889,16 +5357,34 @@
       <c r="AY26">
         <v>0</v>
       </c>
+      <c r="AZ26">
+        <v>10</v>
+      </c>
+      <c r="BA26">
+        <v>1</v>
+      </c>
+      <c r="BB26">
+        <v>1</v>
+      </c>
+      <c r="BC26">
+        <v>0</v>
+      </c>
+      <c r="BD26">
+        <v>0</v>
+      </c>
+      <c r="BE26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:51">
+    <row r="27" spans="1:57">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D27">
         <v>1994</v>
@@ -4985,7 +5471,7 @@
         <v>19</v>
       </c>
       <c r="AF27">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="AG27">
         <v>16</v>
@@ -5033,7 +5519,7 @@
         <v>4.083333333333333</v>
       </c>
       <c r="AV27">
-        <v>47.66666666666666</v>
+        <v>47.70833333333334</v>
       </c>
       <c r="AW27">
         <v>0.6666666666666666</v>
@@ -5044,16 +5530,34 @@
       <c r="AY27">
         <v>3</v>
       </c>
+      <c r="AZ27">
+        <v>21</v>
+      </c>
+      <c r="BA27">
+        <v>11</v>
+      </c>
+      <c r="BB27">
+        <v>6</v>
+      </c>
+      <c r="BC27">
+        <v>3</v>
+      </c>
+      <c r="BD27">
+        <v>0</v>
+      </c>
+      <c r="BE27">
+        <v>3</v>
+      </c>
     </row>
-    <row r="28" spans="1:51">
+    <row r="28" spans="1:57">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D28">
         <v>2011</v>
@@ -5199,16 +5703,34 @@
       <c r="AY28">
         <v>0</v>
       </c>
+      <c r="AZ28">
+        <v>1</v>
+      </c>
+      <c r="BA28">
+        <v>0</v>
+      </c>
+      <c r="BB28">
+        <v>1</v>
+      </c>
+      <c r="BC28">
+        <v>0</v>
+      </c>
+      <c r="BD28">
+        <v>0</v>
+      </c>
+      <c r="BE28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:51">
+    <row r="29" spans="1:57">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D29">
         <v>2006</v>
@@ -5354,16 +5876,34 @@
       <c r="AY29">
         <v>0</v>
       </c>
+      <c r="AZ29">
+        <v>7</v>
+      </c>
+      <c r="BA29">
+        <v>0</v>
+      </c>
+      <c r="BB29">
+        <v>1</v>
+      </c>
+      <c r="BC29">
+        <v>0</v>
+      </c>
+      <c r="BD29">
+        <v>0</v>
+      </c>
+      <c r="BE29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:51">
+    <row r="30" spans="1:57">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D30">
         <v>2011</v>
@@ -5509,16 +6049,34 @@
       <c r="AY30">
         <v>4</v>
       </c>
+      <c r="AZ30">
+        <v>9</v>
+      </c>
+      <c r="BA30">
+        <v>5</v>
+      </c>
+      <c r="BB30">
+        <v>5</v>
+      </c>
+      <c r="BC30">
+        <v>4</v>
+      </c>
+      <c r="BD30">
+        <v>0</v>
+      </c>
+      <c r="BE30">
+        <v>4</v>
+      </c>
     </row>
-    <row r="31" spans="1:51">
+    <row r="31" spans="1:57">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D31">
         <v>2009</v>
@@ -5664,16 +6222,34 @@
       <c r="AY31">
         <v>0</v>
       </c>
+      <c r="AZ31">
+        <v>2</v>
+      </c>
+      <c r="BA31">
+        <v>1</v>
+      </c>
+      <c r="BB31">
+        <v>0</v>
+      </c>
+      <c r="BC31">
+        <v>0</v>
+      </c>
+      <c r="BD31">
+        <v>0</v>
+      </c>
+      <c r="BE31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:51">
+    <row r="32" spans="1:57">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D32">
         <v>1989</v>
@@ -5766,7 +6342,7 @@
         <v>27</v>
       </c>
       <c r="AH32">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="AI32">
         <v>0.06896551724137931</v>
@@ -5819,16 +6395,34 @@
       <c r="AY32">
         <v>12</v>
       </c>
+      <c r="AZ32">
+        <v>37</v>
+      </c>
+      <c r="BA32">
+        <v>30</v>
+      </c>
+      <c r="BB32">
+        <v>14</v>
+      </c>
+      <c r="BC32">
+        <v>12</v>
+      </c>
+      <c r="BD32">
+        <v>2</v>
+      </c>
+      <c r="BE32">
+        <v>14</v>
+      </c>
     </row>
-    <row r="33" spans="1:51">
+    <row r="33" spans="1:57">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C33" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D33">
         <v>2009</v>
@@ -5915,13 +6509,13 @@
         <v>8</v>
       </c>
       <c r="AF33">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AG33">
         <v>7</v>
       </c>
       <c r="AH33">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AI33">
         <v>0.6666666666666666</v>
@@ -5963,7 +6557,7 @@
         <v>3.222222222222222</v>
       </c>
       <c r="AV33">
-        <v>25</v>
+        <v>24.88888888888889</v>
       </c>
       <c r="AW33">
         <v>0.7777777777777778</v>
@@ -5974,16 +6568,34 @@
       <c r="AY33">
         <v>4</v>
       </c>
+      <c r="AZ33">
+        <v>11</v>
+      </c>
+      <c r="BA33">
+        <v>9</v>
+      </c>
+      <c r="BB33">
+        <v>5</v>
+      </c>
+      <c r="BC33">
+        <v>4</v>
+      </c>
+      <c r="BD33">
+        <v>1</v>
+      </c>
+      <c r="BE33">
+        <v>5</v>
+      </c>
     </row>
-    <row r="34" spans="1:51">
+    <row r="34" spans="1:57">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D34">
         <v>1983</v>
@@ -6070,13 +6682,13 @@
         <v>16</v>
       </c>
       <c r="AF34">
-        <v>1425</v>
+        <v>1422</v>
       </c>
       <c r="AG34">
         <v>19</v>
       </c>
       <c r="AH34">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AI34">
         <v>0.08571428571428572</v>
@@ -6118,7 +6730,7 @@
         <v>5.628571428571429</v>
       </c>
       <c r="AV34">
-        <v>40.71428571428572</v>
+        <v>40.62857142857143</v>
       </c>
       <c r="AW34">
         <v>0.5428571428571428</v>
@@ -6129,16 +6741,34 @@
       <c r="AY34">
         <v>2</v>
       </c>
+      <c r="AZ34">
+        <v>24</v>
+      </c>
+      <c r="BA34">
+        <v>21</v>
+      </c>
+      <c r="BB34">
+        <v>3</v>
+      </c>
+      <c r="BC34">
+        <v>2</v>
+      </c>
+      <c r="BD34">
+        <v>0</v>
+      </c>
+      <c r="BE34">
+        <v>2</v>
+      </c>
     </row>
-    <row r="35" spans="1:51">
+    <row r="35" spans="1:57">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D35">
         <v>1984</v>
@@ -6225,13 +6855,13 @@
         <v>1</v>
       </c>
       <c r="AF35">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="AG35">
         <v>20</v>
       </c>
       <c r="AH35">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AI35">
         <v>0</v>
@@ -6273,7 +6903,7 @@
         <v>3.970588235294118</v>
       </c>
       <c r="AV35">
-        <v>33.6764705882353</v>
+        <v>33.70588235294117</v>
       </c>
       <c r="AW35">
         <v>0.5882352941176471</v>
@@ -6284,16 +6914,34 @@
       <c r="AY35">
         <v>0</v>
       </c>
+      <c r="AZ35">
+        <v>7</v>
+      </c>
+      <c r="BA35">
+        <v>2</v>
+      </c>
+      <c r="BB35">
+        <v>0</v>
+      </c>
+      <c r="BC35">
+        <v>0</v>
+      </c>
+      <c r="BD35">
+        <v>0</v>
+      </c>
+      <c r="BE35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:51">
+    <row r="36" spans="1:57">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D36">
         <v>1999</v>
@@ -6380,13 +7028,13 @@
         <v>10</v>
       </c>
       <c r="AF36">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="AG36">
         <v>19</v>
       </c>
       <c r="AH36">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AI36">
         <v>0.2105263157894737</v>
@@ -6428,7 +7076,7 @@
         <v>3.526315789473684</v>
       </c>
       <c r="AV36">
-        <v>59.21052631578947</v>
+        <v>59.26315789473684</v>
       </c>
       <c r="AW36">
         <v>1</v>
@@ -6439,16 +7087,34 @@
       <c r="AY36">
         <v>3</v>
       </c>
+      <c r="AZ36">
+        <v>12</v>
+      </c>
+      <c r="BA36">
+        <v>11</v>
+      </c>
+      <c r="BB36">
+        <v>3</v>
+      </c>
+      <c r="BC36">
+        <v>3</v>
+      </c>
+      <c r="BD36">
+        <v>0</v>
+      </c>
+      <c r="BE36">
+        <v>3</v>
+      </c>
     </row>
-    <row r="37" spans="1:51">
+    <row r="37" spans="1:57">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D37">
         <v>2014</v>
@@ -6535,13 +7201,13 @@
         <v>33</v>
       </c>
       <c r="AF37">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AG37">
         <v>7</v>
       </c>
       <c r="AH37">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AI37">
         <v>0.5</v>
@@ -6583,7 +7249,7 @@
         <v>14.75</v>
       </c>
       <c r="AV37">
-        <v>34</v>
+        <v>33.75</v>
       </c>
       <c r="AW37">
         <v>1.75</v>
@@ -6594,16 +7260,34 @@
       <c r="AY37">
         <v>1</v>
       </c>
+      <c r="AZ37">
+        <v>14</v>
+      </c>
+      <c r="BA37">
+        <v>2</v>
+      </c>
+      <c r="BB37">
+        <v>10</v>
+      </c>
+      <c r="BC37">
+        <v>1</v>
+      </c>
+      <c r="BD37">
+        <v>0</v>
+      </c>
+      <c r="BE37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:51">
+    <row r="38" spans="1:57">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D38">
         <v>2004</v>
@@ -6690,13 +7374,13 @@
         <v>20</v>
       </c>
       <c r="AF38">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="AG38">
         <v>19</v>
       </c>
       <c r="AH38">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AI38">
         <v>0.7142857142857143</v>
@@ -6738,7 +7422,7 @@
         <v>7.5</v>
       </c>
       <c r="AV38">
-        <v>91.64285714285714</v>
+        <v>91.5</v>
       </c>
       <c r="AW38">
         <v>1.357142857142857</v>
@@ -6749,16 +7433,34 @@
       <c r="AY38">
         <v>3</v>
       </c>
+      <c r="AZ38">
+        <v>12</v>
+      </c>
+      <c r="BA38">
+        <v>6</v>
+      </c>
+      <c r="BB38">
+        <v>4</v>
+      </c>
+      <c r="BC38">
+        <v>3</v>
+      </c>
+      <c r="BD38">
+        <v>0</v>
+      </c>
+      <c r="BE38">
+        <v>3</v>
+      </c>
     </row>
-    <row r="39" spans="1:51">
+    <row r="39" spans="1:57">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D39">
         <v>2004</v>
@@ -6845,7 +7547,7 @@
         <v>8</v>
       </c>
       <c r="AF39">
-        <v>1213</v>
+        <v>1208</v>
       </c>
       <c r="AG39">
         <v>18</v>
@@ -6893,7 +7595,7 @@
         <v>6.714285714285714</v>
       </c>
       <c r="AV39">
-        <v>86.64285714285714</v>
+        <v>86.28571428571429</v>
       </c>
       <c r="AW39">
         <v>1.285714285714286</v>
@@ -6904,16 +7606,34 @@
       <c r="AY39">
         <v>1</v>
       </c>
+      <c r="AZ39">
+        <v>8</v>
+      </c>
+      <c r="BA39">
+        <v>7</v>
+      </c>
+      <c r="BB39">
+        <v>1</v>
+      </c>
+      <c r="BC39">
+        <v>1</v>
+      </c>
+      <c r="BD39">
+        <v>0</v>
+      </c>
+      <c r="BE39">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:51">
+    <row r="40" spans="1:57">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C40" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D40">
         <v>2008</v>
@@ -7057,6 +7777,24 @@
         <v>6</v>
       </c>
       <c r="AY40">
+        <v>4</v>
+      </c>
+      <c r="AZ40">
+        <v>14</v>
+      </c>
+      <c r="BA40">
+        <v>6</v>
+      </c>
+      <c r="BB40">
+        <v>5</v>
+      </c>
+      <c r="BC40">
+        <v>4</v>
+      </c>
+      <c r="BD40">
+        <v>0</v>
+      </c>
+      <c r="BE40">
         <v>4</v>
       </c>
     </row>

</xml_diff>